<commit_message>
calcFitness() now *subtracts* the value of exponentialSimilarity() from 1. This way, the better the fit, the closer the value is to 0, and vice versa
</commit_message>
<xml_diff>
--- a/dev1_withGraph.xlsx
+++ b/dev1_withGraph.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/mi21309_bristol_ac_uk/Documents/Documents/Programs/retikulos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="8_{2E7E2FEA-1A55-4C31-8B05-8F6834914817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E29909D8-4359-4D87-A1AF-FC4B8913C7BE}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="8_{2E7E2FEA-1A55-4C31-8B05-8F6834914817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21B91891-248B-4682-A5BC-6B651D3ECD11}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>gene 0</t>
   </si>
@@ -64,6 +64,18 @@
   </si>
   <si>
     <t>index</t>
+  </si>
+  <si>
+    <t>Slope (func)</t>
+  </si>
+  <si>
+    <t>Slope (by hand)</t>
+  </si>
+  <si>
+    <t>expressionStability() result:</t>
+  </si>
+  <si>
+    <t>old func</t>
   </si>
 </sst>
 </file>
@@ -2617,13 +2629,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24:I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
@@ -3005,7 +3020,7 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3029,7 +3044,10 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
       <c r="B18">
         <f>SLOPE(B2:B17,$A$2:$A$17)</f>
         <v>0</v>
@@ -3051,20 +3069,39 @@
         <v>6.6176470588235293E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
       <c r="B19">
-        <f>1-AVERAGE(B18:F18)/MAX(B2:F17)</f>
-        <v>0.99091176470588238</v>
-      </c>
-      <c r="F19" t="s">
-        <v>7</v>
+        <f>(B17-B2)/(15-1)</f>
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <f>(C17-C2)/(15-1)</f>
+        <v>0.21428571428571427</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ref="D19:F19" si="2">(D17-D2)/(15-1)</f>
+        <v>0.35714285714285715</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>2.1428571428571429E-2</v>
       </c>
       <c r="G19">
         <f>STDEV(G2:G17)</f>
         <v>2.5749999999999988</v>
       </c>
+      <c r="H19" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F20" t="s">
         <v>8</v>
       </c>
@@ -3073,7 +3110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F21" t="s">
         <v>9</v>
       </c>
@@ -3082,7 +3119,7 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F22" t="s">
         <v>6</v>
       </c>
@@ -3091,12 +3128,26 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F23" t="s">
         <v>10</v>
       </c>
       <c r="G23">
         <f>G19/(G22)</f>
+        <v>0.24999999999999986</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H25" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25">
+        <f>STDEV(G2:G17)/(MAX(G2:G17)-MIN(G2:G17))</f>
         <v>0.24999999999999986</v>
       </c>
     </row>

</xml_diff>